<commit_message>
changes to ytm calculation (still need to rename spot calculation)
</commit_message>
<xml_diff>
--- a/bond_prices.xlsx
+++ b/bond_prices.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Mathematics\Finance\apm466_assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82F08C4E-C7D6-4AF5-AE8F-7715E19B4ACD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11290BD-B727-483F-9257-84E603FAAB41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{2692AF1C-D5DA-41AA-8319-356DD70C3327}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2692AF1C-D5DA-41AA-8319-356DD70C3327}"/>
   </bookViews>
   <sheets>
     <sheet name="January 6" sheetId="1" r:id="rId1"/>
@@ -520,9 +520,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87E82BAF-90FF-4A1A-993B-DD9D731F0EC3}">
   <dimension ref="A1:Q44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1921,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5C87E3-663B-4BDC-A679-B976BD4F21ED}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K40" sqref="K40"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2006,7 +2004,7 @@
         <v>98.19</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H44" si="0">YEARFRAC("2025-01-07", E3)</f>
+        <f>YEARFRAC("2025-01-07", E3)</f>
         <v>1.4</v>
       </c>
     </row>
@@ -2033,7 +2031,7 @@
         <v>95.89</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H3:H44" si="0">YEARFRAC("2025-01-07", E4)</f>
         <v>2.4</v>
       </c>
     </row>
@@ -3171,8 +3169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DBB2636-CC3B-4ABF-A9CC-90C4A3065D59}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added forward rates and new data
</commit_message>
<xml_diff>
--- a/bond_prices.xlsx
+++ b/bond_prices.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\School\Mathematics\Finance\apm466_assignment_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D313C0-5C8D-4992-98BC-542F3B7620FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13629EDB-BFFF-459D-9929-7409F83BD1BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{2692AF1C-D5DA-41AA-8319-356DD70C3327}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="5" xr2:uid="{2692AF1C-D5DA-41AA-8319-356DD70C3327}"/>
   </bookViews>
   <sheets>
     <sheet name="January 6" sheetId="1" r:id="rId1"/>
     <sheet name="January 7" sheetId="2" r:id="rId2"/>
     <sheet name="January 8" sheetId="3" r:id="rId3"/>
     <sheet name="January 9" sheetId="4" r:id="rId4"/>
+    <sheet name="January 10" sheetId="5" r:id="rId5"/>
+    <sheet name="January 13" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="14">
   <si>
     <t>Canada, Government of...</t>
   </si>
@@ -4420,8 +4422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{645B5654-0696-438F-B9EE-B17EE1031990}">
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5664,4 +5666,2506 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91697EAF-1C1C-4254-B028-051550BBFDFA}">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="E2" s="9">
+        <v>45809</v>
+      </c>
+      <c r="F2" s="7">
+        <v>99.58</v>
+      </c>
+      <c r="G2" s="7">
+        <v>99.66</v>
+      </c>
+      <c r="H2">
+        <f>YEARFRAC("2025-01-10", E2)</f>
+        <v>0.39166666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>46174</v>
+      </c>
+      <c r="F3" s="7">
+        <v>97.95</v>
+      </c>
+      <c r="G3" s="7">
+        <v>98.04</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H44" si="0">YEARFRAC("2025-01-10", E3)</f>
+        <v>1.3916666666666666</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D4" s="8">
+        <v>2.8199999999999999E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>46539</v>
+      </c>
+      <c r="F4" s="7">
+        <v>95.03</v>
+      </c>
+      <c r="G4" s="7">
+        <v>96.06</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>2.3916666666666666</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3.2599999999999997E-2</v>
+      </c>
+      <c r="E5" s="9">
+        <v>45717</v>
+      </c>
+      <c r="F5" s="7">
+        <v>99.7</v>
+      </c>
+      <c r="G5" s="7">
+        <v>99.77</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0.14166666666666666</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>45901</v>
+      </c>
+      <c r="F6" s="7">
+        <v>98.33</v>
+      </c>
+      <c r="G6" s="7">
+        <v>98.41</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.64166666666666672</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>46082</v>
+      </c>
+      <c r="F7" s="7">
+        <v>96.85</v>
+      </c>
+      <c r="G7" s="7">
+        <v>96.93</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.1416666666666666</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>46266</v>
+      </c>
+      <c r="F8" s="7">
+        <v>96.8</v>
+      </c>
+      <c r="G8" s="7">
+        <v>96.88</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>1.6416666666666666</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>46447</v>
+      </c>
+      <c r="F9" s="7">
+        <v>96.33</v>
+      </c>
+      <c r="G9" s="7">
+        <v>96.42</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>2.1416666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>45748</v>
+      </c>
+      <c r="F10" s="7">
+        <v>99.59</v>
+      </c>
+      <c r="G10" s="7">
+        <v>99.67</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.22500000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8">
+        <v>2.75E-2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>2.92E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>46631</v>
+      </c>
+      <c r="F11" s="7">
+        <v>99.21</v>
+      </c>
+      <c r="G11" s="7">
+        <v>99.3</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>2.6416666666666666</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>45931</v>
+      </c>
+      <c r="F12" s="7">
+        <v>99.86</v>
+      </c>
+      <c r="G12" s="7">
+        <v>99.94</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.72499999999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>45689</v>
+      </c>
+      <c r="F13" s="7">
+        <v>99.96</v>
+      </c>
+      <c r="G13" s="7">
+        <v>100.04</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>5.8333333333333334E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3.245E-2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>46623</v>
+      </c>
+      <c r="F14" s="7">
+        <v>100.07</v>
+      </c>
+      <c r="G14" s="7">
+        <v>100.86</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>2.6222222222222222</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D15" s="8">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>46113</v>
+      </c>
+      <c r="F15" s="7">
+        <v>99.87</v>
+      </c>
+      <c r="G15" s="7">
+        <v>99.95</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3.0499999999999999E-2</v>
+      </c>
+      <c r="E16" s="9">
+        <v>45778</v>
+      </c>
+      <c r="F16" s="7">
+        <v>100.14</v>
+      </c>
+      <c r="G16" s="7">
+        <v>100.21</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.30833333333333335</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3.04E-2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>45870</v>
+      </c>
+      <c r="F17" s="7">
+        <v>100.14</v>
+      </c>
+      <c r="G17" s="7">
+        <v>100.22</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.55833333333333335</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E18" s="9">
+        <v>45962</v>
+      </c>
+      <c r="F18" s="7">
+        <v>101.03</v>
+      </c>
+      <c r="G18" s="7">
+        <v>101.13</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.80833333333333335</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>46054</v>
+      </c>
+      <c r="F19" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="G19" s="7">
+        <v>101.48</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>1.0583333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D20" s="8">
+        <v>2.98E-2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>46143</v>
+      </c>
+      <c r="F20" s="7">
+        <v>101.07</v>
+      </c>
+      <c r="G20" s="7">
+        <v>101.31</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>1.3083333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D21" s="8">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="E21" s="9">
+        <v>46237</v>
+      </c>
+      <c r="F21" s="7">
+        <v>101.29</v>
+      </c>
+      <c r="G21" s="7">
+        <v>101.51</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>1.5638888888888889</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>3.245E-2</v>
+      </c>
+      <c r="D22" s="8">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="E22" s="9">
+        <v>46623</v>
+      </c>
+      <c r="F22" s="7">
+        <v>100.07</v>
+      </c>
+      <c r="G22" s="7">
+        <v>100.86</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>2.6222222222222222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="E23" s="9">
+        <v>46054</v>
+      </c>
+      <c r="F23" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="G23" s="7">
+        <v>101.48</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1.0583333333333333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D24" s="8">
+        <v>2.8400000000000002E-2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>46539</v>
+      </c>
+      <c r="F24" s="7">
+        <v>111.19</v>
+      </c>
+      <c r="G24" s="7">
+        <v>111.55</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>2.3916666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D25" s="8">
+        <v>2.8799999999999999E-2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>46174</v>
+      </c>
+      <c r="F25" s="7">
+        <v>97.95</v>
+      </c>
+      <c r="G25" s="7">
+        <v>98.04</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1.3916666666666666</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="D26" s="8">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="E26" s="9">
+        <v>47453</v>
+      </c>
+      <c r="F26" s="7">
+        <v>95.61</v>
+      </c>
+      <c r="G26" s="7">
+        <v>96.47</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>4.8916666666666666</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D27" s="8">
+        <v>2.92E-2</v>
+      </c>
+      <c r="E27" s="9">
+        <v>46813</v>
+      </c>
+      <c r="F27" s="7">
+        <v>101.24</v>
+      </c>
+      <c r="G27" s="7">
+        <v>101.7</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>3.1416666666666666</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D28" s="8">
+        <v>3.32E-2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>48914</v>
+      </c>
+      <c r="F28" s="7">
+        <v>98.57</v>
+      </c>
+      <c r="G28" s="7">
+        <v>99.23</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>8.8916666666666675</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D29" s="8">
+        <v>3.04E-2</v>
+      </c>
+      <c r="E29" s="9">
+        <v>47362</v>
+      </c>
+      <c r="F29" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="G29" s="7">
+        <v>101.66</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>4.6416666666666666</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>2.75E-2</v>
+      </c>
+      <c r="D30" s="8">
+        <v>3.0599999999999999E-2</v>
+      </c>
+      <c r="E30" s="9">
+        <v>47543</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>5.1416666666666666</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D31" s="8">
+        <v>3.1699999999999999E-2</v>
+      </c>
+      <c r="E31" s="9">
+        <v>48000</v>
+      </c>
+      <c r="F31" s="7">
+        <v>89.76</v>
+      </c>
+      <c r="G31" s="7">
+        <v>90.26</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>6.3916666666666666</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D32" s="8">
+        <v>3.1199999999999999E-2</v>
+      </c>
+      <c r="E32" s="9">
+        <v>47818</v>
+      </c>
+      <c r="F32" s="7">
+        <v>85.39</v>
+      </c>
+      <c r="G32" s="7">
+        <v>85.87</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>5.8916666666666666</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D33" s="8">
+        <v>2.9700000000000001E-2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>46997</v>
+      </c>
+      <c r="F33" s="7">
+        <v>100.43</v>
+      </c>
+      <c r="G33" s="7">
+        <v>100.91</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>3.6416666666666666</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D34" s="8">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>49004</v>
+      </c>
+      <c r="F34" s="7">
+        <v>100.7</v>
+      </c>
+      <c r="G34" s="7">
+        <v>101.04</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>9.1416666666666675</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D35" s="8">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>48731</v>
+      </c>
+      <c r="F35" s="7">
+        <v>116.66</v>
+      </c>
+      <c r="G35" s="7">
+        <v>117.58</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>8.3916666666666675</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D36" s="8">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>48366</v>
+      </c>
+      <c r="F36" s="7">
+        <v>91.29</v>
+      </c>
+      <c r="G36" s="7">
+        <v>91.77</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>7.3916666666666666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="8">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D37" s="8">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="E37" s="9">
+        <v>47270</v>
+      </c>
+      <c r="F37" s="7">
+        <v>110.79</v>
+      </c>
+      <c r="G37" s="7">
+        <v>110.99</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>4.3916666666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D38" s="8">
+        <v>3.2099999999999997E-2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>48183</v>
+      </c>
+      <c r="F38" s="7">
+        <v>88.93</v>
+      </c>
+      <c r="G38" s="7">
+        <v>89.39</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>6.8916666666666666</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D39" s="8">
+        <v>3.32E-2</v>
+      </c>
+      <c r="E39" s="9">
+        <v>49096</v>
+      </c>
+      <c r="F39" s="7">
+        <v>96.65</v>
+      </c>
+      <c r="G39" s="7">
+        <v>96.93</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>9.3916666666666675</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D40" s="8">
+        <v>3.32E-2</v>
+      </c>
+      <c r="E40" s="9">
+        <v>49279</v>
+      </c>
+      <c r="F40" s="7">
+        <v>98.35</v>
+      </c>
+      <c r="G40" s="7">
+        <v>98.65</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>9.8916666666666675</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D41" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="E41" s="9">
+        <v>48549</v>
+      </c>
+      <c r="F41" s="7">
+        <v>94.03</v>
+      </c>
+      <c r="G41" s="7">
+        <v>94.51</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>7.8916666666666666</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="D42" s="8">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="E42" s="9">
+        <v>47270</v>
+      </c>
+      <c r="F42" s="7">
+        <v>96.62</v>
+      </c>
+      <c r="G42" s="7">
+        <v>97.08</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>4.3916666666666666</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D43" s="8">
+        <v>2.9899999999999999E-2</v>
+      </c>
+      <c r="E43" s="9">
+        <v>47178</v>
+      </c>
+      <c r="F43" s="7">
+        <v>103.34</v>
+      </c>
+      <c r="G43" s="7">
+        <v>103.6</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>4.1416666666666666</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D44" s="8">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="E44" s="9">
+        <v>46905</v>
+      </c>
+      <c r="F44" s="7">
+        <v>96.62</v>
+      </c>
+      <c r="G44" s="7">
+        <v>96.74</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>3.3916666666666666</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201425-Bond-2025-ca135087d507" xr:uid="{64C4991A-E836-4004-9EA7-1A45A0D530AA}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201526-Bond-2026-ca135087e679" xr:uid="{DCE90D9B-207D-4B0C-A315-F934F1CE7950}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201627-Bond-2027-ca135087f825" xr:uid="{E19CC981-56DF-4527-A38D-6FFE98C2479D}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{80C03308-14E3-450E-A302-B5EC1C044260}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{DF9BE71C-188F-44C4-92AB-41ABD9571195}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{92EFB374-A906-4EA9-9284-4B0463E8D9E1}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{D8C648E8-138B-4E7E-931F-E6F04BAEC59F}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{95B45F4D-BF61-4D04-B39E-B27875BC4C50}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087n340" xr:uid="{A5D250D0-5C0B-4C9F-AE8A-11DF5AE316CA}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{939D8426-745E-48FF-A234-0340E4AA91D1}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{970D0519-8A85-425E-B368-4864DA9AC776}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p659" xr:uid="{5D5C2037-8E57-40DB-A2E8-A699F9F9760C}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087p733" xr:uid="{4B373EF5-BA9C-457D-A557-48497CE99CEE}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202326-Bond-2026-ca135087p816" xr:uid="{24DB75D7-35E4-46C4-842A-9882D0C1BC4D}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325_sq319-Bond-2025-ca135087q319" xr:uid="{CC12D9C5-ABF0-4891-8C80-674381385E1E}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325-Bond-2025-ca135087q640" xr:uid="{59498D09-FC95-4CF5-9294-1336CEF4EBA8}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325-Bond-2025-ca135087q806" xr:uid="{2FF26AC7-A09D-4F7B-B787-8C89FD4BF0BE}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202326-Bond-2026-ca135087r226" xr:uid="{0DBA6CBE-0EB9-49BA-B658-8EE797FD7740}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202426-Bond-2026-ca135087r556" xr:uid="{2918E021-4055-44A2-B11B-46A39BB4CFC9}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202426-Bond-2026-ca135087r978" xr:uid="{BA5D68E0-5880-4D0D-9DB8-5750F38C3E3E}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087p733" xr:uid="{AC2FCDB2-7F91-43BF-826C-0081364D4117}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202326-Bond-2026-ca135087r226" xr:uid="{D8206710-765A-4972-BD1F-2E8834B1FC27}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://markets.businessinsider.com/bonds/8_000-canada-government-of-Bond-2027-ca135087vw17" xr:uid="{FBD2597D-053E-4D85-BCFE-CDE3B09CE304}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201526-Bond-2026-ca135087e679" xr:uid="{33C832E7-69DC-45AE-907E-9862D8A751D4}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202229-Bond-2029-ca135087n670" xr:uid="{4F74195A-603C-4401-983C-5F4CAF266C0E}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{0734E5FB-6237-42D1-A79A-AE783F15FD46}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202333-Bond-2033-ca135087q723" xr:uid="{2C55DDCE-FE6B-48E5-A6FA-F8BE608D0917}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{D3DA29D1-68C1-41A3-B37E-D8F51DA2BF2C}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{D7154105-E63A-40F4-8199-16847B60E960}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202131-Bond-2031-ca135087m276" xr:uid="{76B880BF-66F4-464E-93F3-D4D5DAACF46D}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202030_series_l443-Bond-2030-ca135087l443" xr:uid="{2DD3D186-5A1F-4672-841D-87F069A86A44}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{FF78AA38-36F9-4B28-95B2-5843CEE52A92}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202434-Bond-2034-ca135087r713" xr:uid="{28C384AE-6FFC-4B4F-A338-9436D8799910}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://markets.businessinsider.com/bonds/5_750-canada-government-of-Bond-2033-ca135087xg49" xr:uid="{F3D6A8FB-A793-4E96-ACA2-D68DF07D2AE6}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202232-Bond-2032-ca135087n597" xr:uid="{1AF21B97-3E30-47DD-95BE-F17DD11F70FA}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://markets.businessinsider.com/bonds/5_750-canada-government-of-Bond-2029-ca135087wl43" xr:uid="{A3B62D3B-D80B-47CE-A374-E51E7E1512C7}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202131-Bond-2031-ca135087n266" xr:uid="{FF4044A0-A779-4573-8CBA-4126F65C0A4C}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202334-Bond-2034-ca135087r481" xr:uid="{4B13DBE8-19B8-47BC-A43F-D22368F5273D}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202434-Bond-2034-ca135087s216" xr:uid="{C407CD48-E4CF-4B5C-A726-D796DE531CDF}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202232-Bond-2032-ca135087p329" xr:uid="{7F4DB734-1A77-4B9C-A5D1-2DA8E4D55C51}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201829-Bond-2029-ca135087j397" xr:uid="{BDF6206E-6A0E-44D3-9F8D-5F5E649C4BC1}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{BB6684CD-B035-418A-9633-956AD70FBAD0}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201728-Bond-2028-ca135087h235" xr:uid="{CD8E4663-1FB4-46A6-A7F3-58478A70D838}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId44"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2520D9BC-E33D-40EE-AF1A-9110E8507EB3}">
+  <dimension ref="A1:H44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3.0099999999999998E-2</v>
+      </c>
+      <c r="E2" s="9">
+        <v>46174</v>
+      </c>
+      <c r="F2" s="7">
+        <v>97.95</v>
+      </c>
+      <c r="G2" s="7">
+        <v>98.04</v>
+      </c>
+      <c r="H2">
+        <f>YEARFRAC("2025-01-13", E2)</f>
+        <v>1.3833333333333333</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="E3" s="9">
+        <v>45809</v>
+      </c>
+      <c r="F3" s="7">
+        <v>99.58</v>
+      </c>
+      <c r="G3" s="7">
+        <v>99.66</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H44" si="0">YEARFRAC("2025-01-13", E3)</f>
+        <v>0.38333333333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>3.1600000000000003E-2</v>
+      </c>
+      <c r="E4" s="9">
+        <v>45778</v>
+      </c>
+      <c r="F4" s="7">
+        <v>100.14</v>
+      </c>
+      <c r="G4" s="7">
+        <v>100.21</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E5" s="9">
+        <v>46266</v>
+      </c>
+      <c r="F5" s="7">
+        <v>96.8</v>
+      </c>
+      <c r="G5" s="7">
+        <v>96.88</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>1.6333333333333333</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="D6" s="8">
+        <v>3.09E-2</v>
+      </c>
+      <c r="E6" s="9">
+        <v>46082</v>
+      </c>
+      <c r="F6" s="7">
+        <v>96.85</v>
+      </c>
+      <c r="G6" s="7">
+        <v>96.93</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1.1333333333333333</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E7" s="9">
+        <v>46143</v>
+      </c>
+      <c r="F7" s="7">
+        <v>101.07</v>
+      </c>
+      <c r="G7" s="7">
+        <v>101.31</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>45717</v>
+      </c>
+      <c r="F8" s="7">
+        <v>99.7</v>
+      </c>
+      <c r="G8" s="7">
+        <v>99.77</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8">
+        <v>3.245E-2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2.9499999999999998E-2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>46623</v>
+      </c>
+      <c r="F9" s="7">
+        <v>100.07</v>
+      </c>
+      <c r="G9" s="7">
+        <v>100.86</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>2.6138888888888889</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D10" s="8">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>46113</v>
+      </c>
+      <c r="F10" s="7">
+        <v>99.87</v>
+      </c>
+      <c r="G10" s="7">
+        <v>99.95</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>1.2166666666666666</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>45870</v>
+      </c>
+      <c r="F11" s="7">
+        <v>100.14</v>
+      </c>
+      <c r="G11" s="7">
+        <v>100.22</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>3.0300000000000001E-2</v>
+      </c>
+      <c r="E12" s="9">
+        <v>46447</v>
+      </c>
+      <c r="F12" s="7">
+        <v>96.33</v>
+      </c>
+      <c r="G12" s="7">
+        <v>96.42</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>2.1333333333333333</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="E13" s="9">
+        <v>46419</v>
+      </c>
+      <c r="F13" s="7">
+        <v>99.75</v>
+      </c>
+      <c r="G13" s="7">
+        <v>99.98</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>2.0499999999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D14" s="8">
+        <v>2.9600000000000001E-2</v>
+      </c>
+      <c r="E14" s="9">
+        <v>46539</v>
+      </c>
+      <c r="F14" s="7">
+        <v>95.03</v>
+      </c>
+      <c r="G14" s="7">
+        <v>96.06</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333333</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D15" s="8">
+        <v>3.09E-2</v>
+      </c>
+      <c r="E15" s="9">
+        <v>45962</v>
+      </c>
+      <c r="F15" s="7">
+        <v>101.03</v>
+      </c>
+      <c r="G15" s="7">
+        <v>101.13</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="E16" s="9">
+        <v>46054</v>
+      </c>
+      <c r="F16" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="G16" s="7">
+        <v>101.48</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3.2199999999999999E-2</v>
+      </c>
+      <c r="E17" s="9">
+        <v>45748</v>
+      </c>
+      <c r="F17" s="7">
+        <v>99.59</v>
+      </c>
+      <c r="G17" s="7">
+        <v>99.67</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>0.21666666666666667</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
+        <v>2.75E-2</v>
+      </c>
+      <c r="D18" s="8">
+        <v>3.04E-2</v>
+      </c>
+      <c r="E18" s="9">
+        <v>46631</v>
+      </c>
+      <c r="F18" s="7">
+        <v>99.21</v>
+      </c>
+      <c r="G18" s="7">
+        <v>99.3</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>2.6333333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="D19" s="8">
+        <v>2.9399999999999999E-2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>46539</v>
+      </c>
+      <c r="F19" s="7">
+        <v>111.19</v>
+      </c>
+      <c r="G19" s="7">
+        <v>111.55</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>2.3833333333333333</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>3.1399999999999997E-2</v>
+      </c>
+      <c r="E20" s="9">
+        <v>45901</v>
+      </c>
+      <c r="F20" s="7">
+        <v>98.33</v>
+      </c>
+      <c r="G20" s="7">
+        <v>98.41</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D21" s="8">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="E21" s="9">
+        <v>45931</v>
+      </c>
+      <c r="F21" s="7">
+        <v>99.86</v>
+      </c>
+      <c r="G21" s="7">
+        <v>99.94</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.71666666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D22" s="8">
+        <v>3.09E-2</v>
+      </c>
+      <c r="E22" s="9">
+        <v>45962</v>
+      </c>
+      <c r="F22" s="7">
+        <v>101.03</v>
+      </c>
+      <c r="G22" s="7">
+        <v>101.13</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>3.0700000000000002E-2</v>
+      </c>
+      <c r="E23" s="9">
+        <v>46054</v>
+      </c>
+      <c r="F23" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="G23" s="7">
+        <v>101.48</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" s="8">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="D24" s="8">
+        <v>3.3099999999999997E-2</v>
+      </c>
+      <c r="E24" s="9">
+        <v>45717</v>
+      </c>
+      <c r="F24" s="7">
+        <v>99.7</v>
+      </c>
+      <c r="G24" s="7">
+        <v>99.77</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E25" s="9">
+        <v>46266</v>
+      </c>
+      <c r="F25" s="7">
+        <v>96.8</v>
+      </c>
+      <c r="G25" s="7">
+        <v>96.88</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>1.6333333333333333</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D26" s="8">
+        <v>3.04E-2</v>
+      </c>
+      <c r="E26" s="9">
+        <v>46905</v>
+      </c>
+      <c r="F26" s="7">
+        <v>96.62</v>
+      </c>
+      <c r="G26" s="7">
+        <v>96.74</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>3.3833333333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="E27" s="9">
+        <v>47270</v>
+      </c>
+      <c r="F27" s="7">
+        <v>96.62</v>
+      </c>
+      <c r="G27" s="7">
+        <v>97.08</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>4.3833333333333337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" s="8">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D28" s="8">
+        <v>3.1899999999999998E-2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>47818</v>
+      </c>
+      <c r="F28" s="7">
+        <v>85.39</v>
+      </c>
+      <c r="G28" s="7">
+        <v>85.87</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>5.8833333333333337</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D29" s="8">
+        <v>3.2300000000000002E-2</v>
+      </c>
+      <c r="E29" s="9">
+        <v>48000</v>
+      </c>
+      <c r="F29" s="7">
+        <v>89.76</v>
+      </c>
+      <c r="G29" s="7">
+        <v>90.26</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>6.3833333333333337</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="8">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D30" s="8">
+        <v>3.27E-2</v>
+      </c>
+      <c r="E30" s="9">
+        <v>48183</v>
+      </c>
+      <c r="F30" s="7">
+        <v>88.93</v>
+      </c>
+      <c r="G30" s="7">
+        <v>89.39</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>6.8833333333333337</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="D31" s="8">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E31" s="9">
+        <v>48366</v>
+      </c>
+      <c r="F31" s="7">
+        <v>91.29</v>
+      </c>
+      <c r="G31" s="7">
+        <v>91.77</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>7.3833333333333337</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" s="8">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="D32" s="8">
+        <v>3.09E-2</v>
+      </c>
+      <c r="E32" s="9">
+        <v>47453</v>
+      </c>
+      <c r="F32" s="7">
+        <v>95.61</v>
+      </c>
+      <c r="G32" s="7">
+        <v>96.47</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>4.8833333333333337</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" s="8">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D33" s="8">
+        <v>3.32E-2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>48549</v>
+      </c>
+      <c r="F33" s="7">
+        <v>94.03</v>
+      </c>
+      <c r="G33" s="7">
+        <v>94.51</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>7.8833333333333337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D34" s="8">
+        <v>2.98E-2</v>
+      </c>
+      <c r="E34" s="9">
+        <v>46813</v>
+      </c>
+      <c r="F34" s="7">
+        <v>101.24</v>
+      </c>
+      <c r="G34" s="7">
+        <v>101.7</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>3.1333333333333333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D35" s="8">
+        <v>3.0200000000000001E-2</v>
+      </c>
+      <c r="E35" s="9">
+        <v>46997</v>
+      </c>
+      <c r="F35" s="7">
+        <v>100.43</v>
+      </c>
+      <c r="G35" s="7">
+        <v>100.91</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>3.6333333333333333</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D36" s="8">
+        <v>3.3799999999999997E-2</v>
+      </c>
+      <c r="E36" s="9">
+        <v>48914</v>
+      </c>
+      <c r="F36" s="7">
+        <v>98.57</v>
+      </c>
+      <c r="G36" s="7">
+        <v>99.23</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>8.8833333333333329</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" s="8">
+        <v>0.04</v>
+      </c>
+      <c r="D37" s="8">
+        <v>3.0800000000000001E-2</v>
+      </c>
+      <c r="E37" s="9">
+        <v>47178</v>
+      </c>
+      <c r="F37" s="7">
+        <v>103.34</v>
+      </c>
+      <c r="G37" s="7">
+        <v>103.6</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>4.1333333333333337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C38" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="D38" s="8">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="E38" s="9">
+        <v>49096</v>
+      </c>
+      <c r="F38" s="7">
+        <v>96.65</v>
+      </c>
+      <c r="G38" s="7">
+        <v>96.93</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>9.3833333333333329</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D39" s="8">
+        <v>3.39E-2</v>
+      </c>
+      <c r="E39" s="9">
+        <v>49004</v>
+      </c>
+      <c r="F39" s="7">
+        <v>100.7</v>
+      </c>
+      <c r="G39" s="7">
+        <v>101.04</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>9.1333333333333329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="8">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D40" s="8">
+        <v>3.1300000000000001E-2</v>
+      </c>
+      <c r="E40" s="9">
+        <v>47362</v>
+      </c>
+      <c r="F40" s="7">
+        <v>101.4</v>
+      </c>
+      <c r="G40" s="7">
+        <v>101.66</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>4.6333333333333337</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C41" s="8">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="D41" s="8">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="E41" s="9">
+        <v>49279</v>
+      </c>
+      <c r="F41" s="7">
+        <v>98.35</v>
+      </c>
+      <c r="G41" s="7">
+        <v>98.65</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>9.8833333333333329</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C42" s="8">
+        <v>2.75E-2</v>
+      </c>
+      <c r="D42" s="8">
+        <v>3.1899999999999998E-2</v>
+      </c>
+      <c r="E42" s="9">
+        <v>47543</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>5.1333333333333337</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C43" s="8">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D43" s="8">
+        <v>3.04E-2</v>
+      </c>
+      <c r="E43" s="9">
+        <v>47270</v>
+      </c>
+      <c r="F43" s="7">
+        <v>110.79</v>
+      </c>
+      <c r="G43" s="7">
+        <v>110.99</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>4.3833333333333337</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C44" s="8">
+        <v>5.7500000000000002E-2</v>
+      </c>
+      <c r="D44" s="8">
+        <v>3.3500000000000002E-2</v>
+      </c>
+      <c r="E44" s="9">
+        <v>48731</v>
+      </c>
+      <c r="F44" s="7">
+        <v>116.66</v>
+      </c>
+      <c r="G44" s="7">
+        <v>117.58</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>8.3833333333333329</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201526-Bond-2026-ca135087e679" xr:uid="{986DF955-209F-4B6F-BE98-0F74E9496E1C}"/>
+    <hyperlink ref="A3" r:id="rId2" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201425-Bond-2025-ca135087d507" xr:uid="{0B2CF5DF-C2A0-482E-9816-1F296191FC15}"/>
+    <hyperlink ref="A4" r:id="rId3" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325_sq319-Bond-2025-ca135087q319" xr:uid="{3ACD26DB-3CD9-424E-AA1C-01561CEF55C5}"/>
+    <hyperlink ref="A5" r:id="rId4" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{81E0083E-6D1F-4E4B-B1A1-79D0A51B6BDA}"/>
+    <hyperlink ref="A6" r:id="rId5" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202026-Bond-2026-ca135087l518" xr:uid="{C3415968-DF2A-4465-9883-C1BE9B04042A}"/>
+    <hyperlink ref="A7" r:id="rId6" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202426-Bond-2026-ca135087r556" xr:uid="{6E31C57E-0869-418E-AAE4-F6AD92422EFA}"/>
+    <hyperlink ref="A8" r:id="rId7" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{C85ECBA3-CDC0-4BBA-BF15-1CDF3F93703A}"/>
+    <hyperlink ref="A9" r:id="rId8" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087p733" xr:uid="{7D56956A-B3B4-4230-984B-5E3DD2FC0797}"/>
+    <hyperlink ref="A10" r:id="rId9" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202326-Bond-2026-ca135087p816" xr:uid="{4E970274-6961-4AC5-964E-141E0E28E821}"/>
+    <hyperlink ref="A11" r:id="rId10" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325-Bond-2025-ca135087q640" xr:uid="{36FD0E49-47D7-45DC-B56B-9B77F49671EE}"/>
+    <hyperlink ref="A12" r:id="rId11" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202127-Bond-2027-ca135087m847" xr:uid="{F533C776-5856-4E9F-B0D8-BDBC43F22FE5}"/>
+    <hyperlink ref="A13" r:id="rId12" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202427-Bond-2027-ca135087s547" xr:uid="{50B3CE56-81CE-4E8F-BC42-39BA09391C3A}"/>
+    <hyperlink ref="A14" r:id="rId13" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201627-Bond-2027-ca135087f825" xr:uid="{5164693E-4359-497E-8C37-A7DC4887D74C}"/>
+    <hyperlink ref="A15" r:id="rId14" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325-Bond-2025-ca135087q806" xr:uid="{9060240C-22F4-4672-B015-9DF8D4CC3BBC}"/>
+    <hyperlink ref="A16" r:id="rId15" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202326-Bond-2026-ca135087r226" xr:uid="{76D9D749-AE0F-4092-AAA1-A7DBB66D646F}"/>
+    <hyperlink ref="A17" r:id="rId16" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087n340" xr:uid="{6A1320A9-CAD9-4AD2-B98A-20C83367EBFA}"/>
+    <hyperlink ref="A18" r:id="rId17" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202227-Bond-2027-ca135087n837" xr:uid="{92941994-AB74-4FFB-AA9A-4EF4F1C0186F}"/>
+    <hyperlink ref="A19" r:id="rId18" display="https://markets.businessinsider.com/bonds/8_000-canada-government-of-Bond-2027-ca135087vw17" xr:uid="{8D178721-4BB4-4418-8266-9AE1D196E401}"/>
+    <hyperlink ref="A20" r:id="rId19" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202025-Bond-2025-ca135087k940" xr:uid="{7AD62E8A-116F-47A8-B63E-9B231D844B6E}"/>
+    <hyperlink ref="A21" r:id="rId20" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202225-Bond-2025-ca135087p246" xr:uid="{D0E269B2-97A8-4512-8A38-755E710D9749}"/>
+    <hyperlink ref="A22" r:id="rId21" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202325-Bond-2025-ca135087q806" xr:uid="{5704449E-1142-4B57-B20D-CA4B4FA08811}"/>
+    <hyperlink ref="A23" r:id="rId22" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202326-Bond-2026-ca135087r226" xr:uid="{F2C38B60-A25E-43D5-A5A4-38F9171191C3}"/>
+    <hyperlink ref="A24" r:id="rId23" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201925-Bond-2025-ca135087k528" xr:uid="{C3370BB9-FEF0-4862-BEF4-47A591E080E6}"/>
+    <hyperlink ref="A25" r:id="rId24" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202126-Bond-2026-ca135087l930" xr:uid="{5C64F152-F28D-4B7B-ABAB-E2BC235C9F0A}"/>
+    <hyperlink ref="A26" r:id="rId25" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201728-Bond-2028-ca135087h235" xr:uid="{E95CFC12-AE6D-4C26-BCE0-940A49D4852B}"/>
+    <hyperlink ref="A27" r:id="rId26" display="https://markets.businessinsider.com/bonds/canadacd-bonds_201829-Bond-2029-ca135087j397" xr:uid="{34D313B6-0A01-4510-ABCE-1F56355CA80E}"/>
+    <hyperlink ref="A28" r:id="rId27" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202030_series_l443-Bond-2030-ca135087l443" xr:uid="{146FDAA0-A6C3-44C3-AAA1-F9B1D2E61C48}"/>
+    <hyperlink ref="A29" r:id="rId28" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202131-Bond-2031-ca135087m276" xr:uid="{90A3D241-BBB0-4B14-8E4F-ABD5FFA6476A}"/>
+    <hyperlink ref="A30" r:id="rId29" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202131-Bond-2031-ca135087n266" xr:uid="{514FFB8D-6585-4311-9309-5EA274FE9C67}"/>
+    <hyperlink ref="A31" r:id="rId30" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202232-Bond-2032-ca135087n597" xr:uid="{6BC0A921-B046-4A9A-BFF2-B345E2336520}"/>
+    <hyperlink ref="A32" r:id="rId31" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202229-Bond-2029-ca135087n670" xr:uid="{333C3E00-6D0A-4B36-86F2-F1B61DBB96E0}"/>
+    <hyperlink ref="A33" r:id="rId32" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202232-Bond-2032-ca135087p329" xr:uid="{9A3B045A-065A-4AA9-A734-636B06DD0718}"/>
+    <hyperlink ref="A34" r:id="rId33" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202228-Bond-2028-ca135087p576" xr:uid="{EE71460D-5013-4481-9C42-E5FD28598F5F}"/>
+    <hyperlink ref="A35" r:id="rId34" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202328-Bond-2028-ca135087q491" xr:uid="{66D4F4F1-539F-402D-A707-F03C5CA62B05}"/>
+    <hyperlink ref="A36" r:id="rId35" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202333-Bond-2033-ca135087q723" xr:uid="{7D41FE8C-134D-445D-BF25-7A2789674056}"/>
+    <hyperlink ref="A37" r:id="rId36" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202329-Bond-2029-ca135087q988" xr:uid="{9240B12E-B95A-495F-8364-DAFA97A385E9}"/>
+    <hyperlink ref="A38" r:id="rId37" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202334-Bond-2034-ca135087r481" xr:uid="{7E3DC4DF-1F1A-4ABF-84E0-3394D1F8EBAB}"/>
+    <hyperlink ref="A39" r:id="rId38" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202434-Bond-2034-ca135087r713" xr:uid="{B8E7A867-FF97-47F4-95CE-97C19E9B9568}"/>
+    <hyperlink ref="A40" r:id="rId39" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202429-Bond-2029-ca135087r895" xr:uid="{D9728C38-158C-4BCA-89EE-489BC3304893}"/>
+    <hyperlink ref="A41" r:id="rId40" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202434-Bond-2034-ca135087s216" xr:uid="{88AF5983-1C0D-4065-BF2F-287E6EAC1BF4}"/>
+    <hyperlink ref="A42" r:id="rId41" display="https://markets.businessinsider.com/bonds/canadacd-bonds_202430-Bond-2030-ca135087s471" xr:uid="{80E2C71E-D65D-47B0-9EC8-12EC271B5AEB}"/>
+    <hyperlink ref="A43" r:id="rId42" display="https://markets.businessinsider.com/bonds/5_750-canada-government-of-Bond-2029-ca135087wl43" xr:uid="{56702D30-736D-4445-BBCA-60799470531F}"/>
+    <hyperlink ref="A44" r:id="rId43" display="https://markets.businessinsider.com/bonds/5_750-canada-government-of-Bond-2033-ca135087xg49" xr:uid="{61D0BD00-6476-4B2B-9692-F68C0D803D78}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>